<commit_message>
Creacion DB, correccion relaciones, sync db.
</commit_message>
<xml_diff>
--- a/proyecto-sin-nombre-definido/MockData/MockData.xlsx
+++ b/proyecto-sin-nombre-definido/MockData/MockData.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16155" windowHeight="4860"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16155" windowHeight="4860" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Base" sheetId="1" r:id="rId1"/>
+    <sheet name="Ejemplo datos" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="93">
   <si>
     <t>Mock data</t>
   </si>
@@ -92,18 +93,9 @@
     <t xml:space="preserve">history </t>
   </si>
   <si>
-    <t>objeto</t>
-  </si>
-  <si>
     <t>(tentativo)</t>
   </si>
   <si>
-    <t>JSON.stringify(var)</t>
-  </si>
-  <si>
-    <t>trabajamos con json porque no existe un dataType de objeto</t>
-  </si>
-  <si>
     <t>historial de contratos/casas alquiladas</t>
   </si>
   <si>
@@ -161,9 +153,6 @@
     <t>text</t>
   </si>
   <si>
-    <t>array(integer)</t>
-  </si>
-  <si>
     <t>integer</t>
   </si>
   <si>
@@ -246,13 +235,86 @@
   </si>
   <si>
     <t>landlord</t>
+  </si>
+  <si>
+    <t>temporal</t>
+  </si>
+  <si>
+    <t>Template para back-end</t>
+  </si>
+  <si>
+    <t>Revisar abajo la pestaña de ejemplo para manejo en front</t>
+  </si>
+  <si>
+    <t>Messi2023</t>
+  </si>
+  <si>
+    <t>Lionel Messi</t>
+  </si>
+  <si>
+    <t>https://assets.goal.com/v3/assets/bltcc7a7ffd2fbf71f5/blt9210c8d5e9b04af3/615f75d1f0cc0276fbb26d71/d27b847732f6968d3ec83e569617ab16ae0f7af9.jpg?auto=webp&amp;format=pjpg&amp;width=3840&amp;quality=60</t>
+  </si>
+  <si>
+    <t>11 0303 4560</t>
+  </si>
+  <si>
+    <t>11 0404 5670</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Calle falsa 123</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>leo.messi@yahoo.com</t>
+  </si>
+  <si>
+    <t>trescopas</t>
+  </si>
+  <si>
+    <t>El Wilderness Hotel Inari &amp; Igloos, situado a orillas del lago Inari, ofrece alojamiento y actividades. El hotel, que se inspira en la cultura lapona, tiene sauna y salón compartido con bar.
+Se puede elegir entre la cabaña con vistas al cielo para ver las auroras, la cabaña de madera con vistas al lago Inari o la habitación Wilderness con elementos decorativos lapones. Todas las habitaciones disponen de un baño con artículos de aseo. Algunas habitaciones disponen de sauna y TV de pantalla plana.
+Se sirve un desayuno buffet a diario. El restaurante Ukko, de temática lapona, ofrece vistas panorámicas del lago Inari.
+El Wilderness Hotel Inari &amp; Igloos propone una variedad de actividades, como paseos con huskies, esquí de fondo, visitas a granjas de renos, pesca en el hielo y observación de auroras.
+El Wilderness Hotel Inari &amp; Igloos se encuentra a 5 minutos en auto del pueblo de Inari. El aeropuerto de Ivalo está a 47 km.</t>
+  </si>
+  <si>
+    <t>Inarintie 2, 99870 Inari, Finlandia</t>
+  </si>
+  <si>
+    <t>Finland</t>
+  </si>
+  <si>
+    <t>https://cf.bstatic.com/xdata/images/hotel/max1024x768/250776827.jpg?k=00616da8783983917c7fe8e0ca8251d8b09535accb5b4bf85cbee6a11202bdbf&amp;o=&amp;hp=1</t>
+  </si>
+  <si>
+    <t>2 imágenes para usar de array</t>
+  </si>
+  <si>
+    <t>https://cf.bstatic.com/xdata/images/hotel/max1024x768/182686134.jpg?k=cb49283a363e3533f4a05a3e4f35077ef4aa88a2432262cecf662c4844eb41af&amp;o=&amp;hp=1</t>
+  </si>
+  <si>
+    <t>rentPrice</t>
+  </si>
+  <si>
+    <t>sellPrice</t>
+  </si>
+  <si>
+    <t>usd/night</t>
+  </si>
+  <si>
+    <t>Provincia de Buenos Aires</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -276,6 +338,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF262626"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -285,7 +369,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -293,17 +377,63 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -582,10 +712,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,201 +724,189 @@
     <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="2:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B1" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B2" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>8</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>10</v>
       </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>11</v>
       </c>
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>12</v>
-      </c>
-      <c r="C11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>15</v>
       </c>
       <c r="C13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>16</v>
       </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" t="s">
-        <v>18</v>
-      </c>
       <c r="C16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" t="s">
-        <v>24</v>
-      </c>
-      <c r="F16" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>73</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" t="s">
         <v>23</v>
       </c>
-      <c r="B18" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" t="s">
-        <v>29</v>
-      </c>
-      <c r="F19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C25" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>31</v>
-      </c>
-      <c r="C25" t="s">
-        <v>5</v>
-      </c>
-    </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" t="s">
-        <v>44</v>
-      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="C27" t="s">
         <v>5</v>
@@ -796,15 +914,15 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="C29" t="s">
         <v>5</v>
@@ -812,229 +930,253 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C30" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C31" t="s">
-        <v>19</v>
-      </c>
-      <c r="E31" t="s">
-        <v>48</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C32" t="s">
-        <v>45</v>
-      </c>
-      <c r="E32" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C33" t="s">
-        <v>46</v>
+        <v>19</v>
+      </c>
+      <c r="E33" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>39</v>
+        <v>89</v>
       </c>
       <c r="C34" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="C35" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E35" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C36" t="s">
-        <v>47</v>
-      </c>
-      <c r="E36" t="s">
-        <v>49</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>51</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
+        <v>37</v>
+      </c>
+      <c r="C38" t="s">
+        <v>43</v>
+      </c>
+      <c r="E38" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>42</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" t="s">
         <v>43</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
+      <c r="E39" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>47</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>39</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B43" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C43" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B44" s="2" t="s">
+      <c r="B43" t="s">
+        <v>40</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B46" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C46" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B47" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C47" s="2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>56</v>
-      </c>
-      <c r="C45" t="s">
-        <v>5</v>
-      </c>
-      <c r="D45" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>57</v>
-      </c>
-      <c r="C46" t="s">
-        <v>5</v>
-      </c>
-      <c r="D46" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>59</v>
-      </c>
-      <c r="C47" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C48" t="s">
-        <v>64</v>
+        <v>5</v>
+      </c>
+      <c r="D48" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C49" t="s">
-        <v>63</v>
+        <v>5</v>
+      </c>
+      <c r="D49" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C50" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="C51" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C52" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>23</v>
-      </c>
       <c r="B53" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C53" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="C54" t="s">
-        <v>19</v>
-      </c>
-      <c r="E54" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C55" t="s">
-        <v>5</v>
-      </c>
-      <c r="E55" t="s">
-        <v>71</v>
+        <v>19</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>22</v>
+      </c>
       <c r="B56" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C56" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>64</v>
+      </c>
+      <c r="C57" t="s">
+        <v>19</v>
+      </c>
+      <c r="E57" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>66</v>
+      </c>
+      <c r="C58" t="s">
+        <v>5</v>
+      </c>
+      <c r="E58" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>68</v>
+      </c>
+      <c r="C59" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1042,4 +1184,355 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="6">
+        <v>29221</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B27" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="8"/>
+      <c r="C31" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="8"/>
+      <c r="C32" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" t="b">
+        <v>1</v>
+      </c>
+      <c r="E33" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34">
+        <v>100</v>
+      </c>
+      <c r="D34" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C35">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38">
+        <v>87.6</v>
+      </c>
+      <c r="E38" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39">
+        <v>300</v>
+      </c>
+      <c r="E39" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>47</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>39</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>40</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B46" s="1"/>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C7" r:id="rId1"/>
+    <hyperlink ref="C14" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Correccion post asset controller
</commit_message>
<xml_diff>
--- a/proyecto-sin-nombre-definido/MockData/MockData.xlsx
+++ b/proyecto-sin-nombre-definido/MockData/MockData.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="97">
   <si>
     <t>Mock data</t>
   </si>
@@ -308,6 +308,18 @@
   </si>
   <si>
     <t>Provincia de Buenos Aires</t>
+  </si>
+  <si>
+    <t>Asset 3</t>
+  </si>
+  <si>
+    <t>81db66f5-2260-4bdb-a17b-fd73740bfc62</t>
+  </si>
+  <si>
+    <t>Asset 2</t>
+  </si>
+  <si>
+    <t>f41a19f2-04b4-4c9c-850c-97a9782e347e</t>
   </si>
 </sst>
 </file>
@@ -1188,10 +1200,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1410,7 +1422,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B31" s="8"/>
-      <c r="C31" t="s">
+      <c r="C31" s="5" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1528,10 +1540,27 @@
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
     </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>96</v>
+      </c>
+      <c r="C48" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>94</v>
+      </c>
+      <c r="C49" t="s">
+        <v>93</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C7" r:id="rId1"/>
     <hyperlink ref="C14" r:id="rId2"/>
+    <hyperlink ref="C31" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>